<commit_message>
Evaluate similarity als to best optimal order
</commit_message>
<xml_diff>
--- a/data/data_prepared.xlsx
+++ b/data/data_prepared.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="54">
   <si>
     <t>ProbandID</t>
   </si>
@@ -139,6 +139,12 @@
     <t>True error</t>
   </si>
   <si>
+    <t>to proposed order</t>
+  </si>
+  <si>
+    <t>to closest optimal order</t>
+  </si>
+  <si>
     <t>LTQ1A</t>
   </si>
   <si>
@@ -182,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -192,9 +198,10 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <name val="Arial"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,10 +274,10 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,14 +1236,14 @@
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="5" t="s">
         <v>51</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -18932,7 +18939,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="3" width="12.86"/>
+    <col customWidth="1" min="2" max="2" width="16.29"/>
+    <col customWidth="1" min="3" max="4" width="12.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -18940,9 +18948,12 @@
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -18950,144 +18961,443 @@
       <c r="A2" s="8">
         <v>2.0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="14">
         <v>0.8</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D2" s="14">
         <v>0.4</v>
       </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3">
       <c r="A3" s="8">
         <v>3.0</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="14">
         <v>0.8</v>
       </c>
-      <c r="C3" s="8">
+      <c r="D3" s="14">
         <v>0.3</v>
       </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4">
       <c r="A4" s="8">
         <v>4.0</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="14">
         <v>0.8</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D4" s="14">
         <v>0.2</v>
       </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5">
       <c r="A5" s="8">
         <v>5.0</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="14">
         <v>0.8</v>
       </c>
-      <c r="C5" s="8">
+      <c r="D5" s="14">
         <v>0.5</v>
       </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6">
       <c r="A6" s="8">
         <v>6.0</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="14">
         <v>0.6</v>
       </c>
-      <c r="C6" s="8">
+      <c r="D6" s="14">
         <v>0.3</v>
       </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7">
       <c r="A7" s="8">
         <v>7.0</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="14">
         <v>0.8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="D7" s="14">
         <v>0.7</v>
       </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8">
       <c r="A8" s="8">
         <v>8.0</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="14">
         <v>0.8</v>
       </c>
-      <c r="C8" s="8">
+      <c r="D8" s="14">
         <v>0.4</v>
       </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9">
       <c r="A9" s="8">
         <v>9.0</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="14">
         <v>0.6</v>
       </c>
-      <c r="C9" s="8">
+      <c r="D9" s="14">
         <v>0.3</v>
       </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10">
       <c r="A10" s="8">
         <v>10.0</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="14">
         <v>0.8</v>
       </c>
-      <c r="C10" s="8">
+      <c r="D10" s="14">
         <v>0.5</v>
       </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="8">
         <v>11.0</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="14">
         <v>0.6</v>
       </c>
-      <c r="C11" s="8">
+      <c r="D11" s="14">
         <v>0.3</v>
       </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12">
       <c r="A12" s="8">
         <v>12.0</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="14">
         <v>0.8</v>
       </c>
-      <c r="C12" s="8">
+      <c r="D12" s="14">
         <v>0.3</v>
       </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13">
       <c r="A13" s="8">
         <v>13.0</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14">
         <v>0.8</v>
       </c>
-      <c r="C13" s="8">
+      <c r="D13" s="14">
         <v>0.4</v>
       </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14">
       <c r="A14" s="8">
         <v>14.0</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="14">
         <v>0.2</v>
       </c>
-      <c r="C14" s="8">
+      <c r="D14" s="14">
         <v>0.3</v>
       </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="D27" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -19108,14 +19418,14 @@
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -19319,30 +19629,30 @@
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="G1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" s="8">
@@ -19683,34 +19993,34 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="15"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="15"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="15"/>
+      <c r="A22" s="5"/>
     </row>
     <row r="23">
-      <c r="A23" s="15"/>
+      <c r="A23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="15"/>
+      <c r="A24" s="5"/>
     </row>
     <row r="25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="5"/>
     </row>
     <row r="26">
-      <c r="A26" s="15"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27">
-      <c r="A27" s="15"/>
+      <c r="A27" s="5"/>
     </row>
     <row r="28">
-      <c r="A28" s="15"/>
+      <c r="A28" s="5"/>
     </row>
     <row r="29">
-      <c r="A29" s="15"/>
+      <c r="A29" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>